<commit_message>
Added DY amcanlo info
</commit_message>
<xml_diff>
--- a/pdf_sets.xlsx
+++ b/pdf_sets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="94">
   <si>
     <t>/tZq_ll_4f_13TeV-amcatnlo-pythia8/RunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6_ext1-v1/MINIAODSIM</t>
   </si>
@@ -401,13 +401,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1439,8 +1439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="C21" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34:I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2337,42 +2337,102 @@
       <c r="A32" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="4">
         <v>28968252</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="4">
         <v>5765.4</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="5"/>
-      <c r="C33" s="6">
+      <c r="E32">
+        <v>292200</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" t="s">
+        <v>80</v>
+      </c>
+      <c r="H32" t="s">
+        <v>82</v>
+      </c>
+      <c r="I32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="6"/>
+      <c r="C33" s="4">
         <v>122055388</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>292200</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" t="s">
+        <v>80</v>
+      </c>
+      <c r="H33" t="s">
+        <v>82</v>
+      </c>
+      <c r="I33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="4">
         <v>65888233</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="4">
         <v>18610</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>292200</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" t="s">
+        <v>80</v>
+      </c>
+      <c r="H34" t="s">
+        <v>82</v>
+      </c>
+      <c r="I34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="4">
         <v>40381391</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>292200</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G35" t="s">
+        <v>80</v>
+      </c>
+      <c r="H35" t="s">
+        <v>82</v>
+      </c>
+      <c r="I35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>93</v>
       </c>
@@ -2420,10 +2480,14 @@
     <hyperlink ref="B34" r:id="rId36" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FDYJetsToLL_M-50_TuneCUETP8M1_13TeV-amcatnloFXFX-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6_ext2-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
     <hyperlink ref="B35" r:id="rId37" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FDYJetsToLL_M-10to50_TuneCUETP8M1_13TeV-amcatnloFXFX-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v2%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
     <hyperlink ref="B36" r:id="rId38" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FDYJetsToLL_M-10to50_TuneCUETP8M1_13TeV-amcatnloFXFX-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6_ext1-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
+    <hyperlink ref="F32" r:id="rId39"/>
+    <hyperlink ref="F33" r:id="rId40"/>
+    <hyperlink ref="F34" r:id="rId41"/>
+    <hyperlink ref="F35" r:id="rId42"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId39"/>
-  <drawing r:id="rId40"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId43"/>
+  <drawing r:id="rId44"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated the pdf sets used.
</commit_message>
<xml_diff>
--- a/pdf_sets.xlsx
+++ b/pdf_sets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="4905" windowWidth="25605" windowHeight="17535" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="112">
   <si>
     <t>/tZq_ll_4f_13TeV-amcatnlo-pythia8/RunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6_ext1-v1/MINIAODSIM</t>
   </si>
@@ -306,6 +306,60 @@
   </si>
   <si>
     <t>/DYJetsToLL_M-10to50_TuneCUETP8M1_13TeV-amcatnloFXFX-pythia8/RunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6_ext1-v1/MINIAODSIM</t>
+  </si>
+  <si>
+    <t>FCNC:</t>
+  </si>
+  <si>
+    <t>tZq -&gt; lll</t>
+  </si>
+  <si>
+    <t>tZq -&gt; ll</t>
+  </si>
+  <si>
+    <t>/ST_FCNC-TLL_Thadronic_zeta_zct-MadGraph5-pythia8/RunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1/MINIAODSIM</t>
+  </si>
+  <si>
+    <t>/ST_FCNC-TLL_Thadronic_kappa_zut-MadGraph5-pythia8/RunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1/MINIAODSIM</t>
+  </si>
+  <si>
+    <t>/ST_FCNC-TLL_Thadronic_zeta_zut-MadGraph5-pythia8/RunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1/MINIAODSIM</t>
+  </si>
+  <si>
+    <t>/ST_FCNC-TLL_Thadronic_kappa_zct-MadGraph5-pythia8/RunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1/MINIAODSIM</t>
+  </si>
+  <si>
+    <t>NNPDF23_lo_as_0130_qed</t>
+  </si>
+  <si>
+    <t>/ST_FCNC-TLL_Tleptonic_zeta_zct-MadGraph5-pythia8/RunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1/MINIAODSIM</t>
+  </si>
+  <si>
+    <t>/ST_FCNC-TLL_Tleptonic_kappa_zct-MadGraph5-pythia8/RunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1/MINIAODSIM</t>
+  </si>
+  <si>
+    <t>/ST_FCNC-TLL_Tleptonic_zeta_zut-MadGraph5-pythia8/RunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1/MINIAODSIM</t>
+  </si>
+  <si>
+    <t>/ST_FCNC-TLL_Tleptonic_kappa_zut-MadGraph5-pythia8/RunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1/MINIAODSIM</t>
+  </si>
+  <si>
+    <t>214-314</t>
+  </si>
+  <si>
+    <t>TTbar</t>
+  </si>
+  <si>
+    <t>tZq (Z -&gt; Hadronic)</t>
+  </si>
+  <si>
+    <t>/tZq_W_lept_Z_hadron_4f_ckm_NLO_13TeV_amcatnlo_pythia8/RunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1/MINIAODSIM</t>
+  </si>
+  <si>
+    <t>1111-1112</t>
+  </si>
+  <si>
+    <t>1011-1110</t>
   </si>
 </sst>
 </file>
@@ -432,13 +486,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -489,13 +543,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -546,13 +600,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -603,13 +657,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -660,76 +714,19 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1029" name="Picture 5" descr="//twiki.cern.ch/twiki/pub/TWiki/TWikiDocGraphics/external-link.gif">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4" tgtFrame="_blank"/>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1590675" y="2200275"/>
-          <a:ext cx="123825" cy="114300"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1030" name="Picture 6" descr="//twiki.cern.ch/twiki/pub/TWiki/TWikiDocGraphics/external-link.gif">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5" tgtFrame="_blank"/>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
@@ -785,6 +782,63 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
+        <xdr:cNvPr id="1030" name="Picture 6" descr="//twiki.cern.ch/twiki/pub/TWiki/TWikiDocGraphics/external-link.gif">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5" tgtFrame="_blank"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1590675" y="2200275"/>
+          <a:ext cx="123825" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
         <xdr:cNvPr id="1031" name="Picture 7" descr="//twiki.cern.ch/twiki/pub/TWiki/TWikiDocGraphics/external-link.gif">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6" tgtFrame="_blank"/>
         </xdr:cNvPr>
@@ -831,13 +885,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -888,13 +942,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -945,13 +999,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1002,13 +1056,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1059,13 +1113,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1093,6 +1147,120 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="1590675" y="7019925"/>
+          <a:ext cx="123825" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13" descr="https://twiki.cern.ch/twiki/pub/TWiki/TWikiDocGraphics/external-link.gif">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12" tgtFrame="_blank"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1590675" y="8020050"/>
+          <a:ext cx="123825" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14" descr="https://twiki.cern.ch/twiki/pub/TWiki/TWikiDocGraphics/external-link.gif">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13" tgtFrame="_blank"/>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1590675" y="400050"/>
           <a:ext cx="123825" cy="114300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1437,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34:I35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1515,57 +1683,51 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>3496799</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
+        <v>108</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="E3">
-        <v>263400</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>85</v>
+        <v>292000</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>80</v>
       </c>
       <c r="H3" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="I3" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>50000</v>
+        <v>3496799</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="E4">
-        <v>263000</v>
+        <v>263400</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>85</v>
       </c>
       <c r="H4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I4" t="s">
         <v>87</v>
@@ -1573,39 +1735,42 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>50000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>263000</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>1992438</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5">
-        <v>292200</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>5982673</v>
       </c>
       <c r="D6" t="s">
         <v>41</v>
@@ -1628,13 +1793,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7">
-        <v>749400</v>
+        <v>5982673</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="E7">
         <v>292200</v>
@@ -1653,17 +1818,14 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>42</v>
+      <c r="B8" t="s">
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>2160168</v>
+        <v>749400</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="E8">
         <v>292200</v>
@@ -1682,11 +1844,14 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>43</v>
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C9">
-        <v>2000000</v>
+        <v>2160168</v>
       </c>
       <c r="D9" t="s">
         <v>45</v>
@@ -1708,14 +1873,14 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>44</v>
+      <c r="B10" t="s">
+        <v>43</v>
       </c>
       <c r="C10">
-        <v>833298</v>
+        <v>2000000</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E10">
         <v>292200</v>
@@ -1734,43 +1899,43 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
       <c r="B11" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11">
-        <v>49748967</v>
+        <v>833298</v>
       </c>
       <c r="D11" t="s">
         <v>36</v>
       </c>
       <c r="E11">
-        <v>263000</v>
+        <v>292200</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H11" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="I11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
       <c r="B12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12">
-        <v>96821363</v>
-      </c>
-      <c r="D12">
-        <v>4895</v>
+        <v>49748967</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
       </c>
       <c r="E12">
         <v>263000</v>
@@ -1790,13 +1955,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13">
-        <v>35307372</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
+        <v>96821363</v>
+      </c>
+      <c r="D13">
+        <v>4895</v>
       </c>
       <c r="E13">
         <v>263000</v>
@@ -1815,46 +1980,43 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>49</v>
+      <c r="B14" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="C14">
-        <v>24222907</v>
+        <v>35307372</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E14">
-        <v>292200</v>
+        <v>263000</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G14" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H14" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="I14" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C15">
-        <v>1999000</v>
+        <v>24222907</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="E15">
         <v>292200</v>
@@ -1874,13 +2036,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16">
-        <v>1999200</v>
+        <v>1999000</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
@@ -1902,14 +2064,17 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>54</v>
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
       </c>
       <c r="C17">
-        <v>6998600</v>
+        <v>1999200</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="E17">
         <v>292200</v>
@@ -1928,17 +2093,14 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s">
-        <v>56</v>
+      <c r="B18" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="C18">
-        <v>1960761</v>
+        <v>6998600</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E18">
         <v>292200</v>
@@ -1958,16 +2120,16 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19">
-        <v>26533019</v>
+        <v>1960761</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="E19">
         <v>292200</v>
@@ -1987,13 +2149,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20">
-        <v>-1</v>
+        <v>26533019</v>
       </c>
       <c r="D20" t="s">
         <v>36</v>
@@ -2016,16 +2178,16 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21">
-        <v>10723190</v>
+        <v>-1</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="E21">
         <v>292200</v>
@@ -2045,16 +2207,16 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C22">
-        <v>8992075</v>
+        <v>10723190</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E22">
         <v>292200</v>
@@ -2074,16 +2236,16 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23">
-        <v>15537011</v>
+        <v>8992075</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="E23">
         <v>292200</v>
@@ -2103,39 +2265,42 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24">
-        <v>6105137</v>
+        <v>15537011</v>
       </c>
       <c r="D24" t="s">
         <v>36</v>
       </c>
       <c r="E24">
-        <v>263000</v>
+        <v>292200</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G24" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H24" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="I24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25">
-        <v>24767666</v>
+        <v>6105137</v>
       </c>
       <c r="D25" t="s">
         <v>36</v>
@@ -2157,55 +2322,49 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>16</v>
-      </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C26">
-        <v>77615423</v>
-      </c>
-      <c r="D26">
-        <v>730</v>
+        <v>24767666</v>
+      </c>
+      <c r="D26" t="s">
+        <v>36</v>
       </c>
       <c r="E26">
-        <v>260000</v>
+        <v>263000</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="G26" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H26" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="I26" t="s">
-        <v>84</v>
-      </c>
-      <c r="J26" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C27">
-        <v>6952830</v>
-      </c>
-      <c r="D27" t="s">
-        <v>71</v>
+        <v>77615423</v>
+      </c>
+      <c r="D27">
+        <v>730</v>
       </c>
       <c r="E27">
-        <v>292200</v>
+        <v>260000</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="G27" t="s">
         <v>80</v>
@@ -2216,16 +2375,19 @@
       <c r="I27" t="s">
         <v>84</v>
       </c>
+      <c r="J27" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C28">
-        <v>6971574</v>
+        <v>6952830</v>
       </c>
       <c r="D28" t="s">
         <v>71</v>
@@ -2248,22 +2410,22 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29">
-        <v>1000000</v>
+        <v>6971574</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E29">
-        <v>292000</v>
-      </c>
-      <c r="F29" t="s">
-        <v>35</v>
+        <v>292200</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G29" t="s">
         <v>80</v>
@@ -2277,16 +2439,16 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>75</v>
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
+        <v>73</v>
       </c>
       <c r="C30">
-        <v>67250880</v>
+        <v>1000000</v>
       </c>
       <c r="D30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E30">
         <v>292000</v>
@@ -2304,18 +2466,18 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C31">
-        <v>38811017</v>
+        <v>67250880</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E31">
         <v>292000</v>
@@ -2333,24 +2495,24 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>89</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" s="4">
-        <v>28968252</v>
-      </c>
-      <c r="D32" s="4">
-        <v>5765.4</v>
+        <v>34</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32">
+        <v>38811017</v>
+      </c>
+      <c r="D32" t="s">
+        <v>78</v>
       </c>
       <c r="E32">
-        <v>292200</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>38</v>
+        <v>292000</v>
+      </c>
+      <c r="F32" t="s">
+        <v>35</v>
       </c>
       <c r="G32" t="s">
         <v>80</v>
@@ -2362,10 +2524,18 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="6"/>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="C33" s="4">
-        <v>122055388</v>
+        <v>28968252</v>
+      </c>
+      <c r="D33" s="4">
+        <v>5765.4</v>
       </c>
       <c r="E33">
         <v>292200</v>
@@ -2383,15 +2553,10 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
-        <v>91</v>
-      </c>
+    <row r="34" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="6"/>
       <c r="C34" s="4">
-        <v>65888233</v>
-      </c>
-      <c r="D34" s="4">
-        <v>18610</v>
+        <v>122055388</v>
       </c>
       <c r="E34">
         <v>292200</v>
@@ -2409,12 +2574,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C35" s="4">
-        <v>40381391</v>
+        <v>65888233</v>
+      </c>
+      <c r="D35" s="4">
+        <v>18610</v>
       </c>
       <c r="E35">
         <v>292200</v>
@@ -2432,62 +2600,307 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="4">
+        <v>40381391</v>
+      </c>
+      <c r="E36">
+        <v>292200</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G36" t="s">
+        <v>80</v>
+      </c>
+      <c r="H36" t="s">
+        <v>82</v>
+      </c>
+      <c r="I36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
         <v>93</v>
+      </c>
+      <c r="E37">
+        <v>292200</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="4">
+        <v>1912224</v>
+      </c>
+      <c r="E39">
+        <v>230000</v>
+      </c>
+      <c r="F39" t="s">
+        <v>101</v>
+      </c>
+      <c r="G39" t="s">
+        <v>85</v>
+      </c>
+      <c r="H39" t="s">
+        <v>106</v>
+      </c>
+      <c r="I39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="4">
+        <v>1992044</v>
+      </c>
+      <c r="E40">
+        <v>230000</v>
+      </c>
+      <c r="F40" t="s">
+        <v>101</v>
+      </c>
+      <c r="G40" t="s">
+        <v>85</v>
+      </c>
+      <c r="H40" t="s">
+        <v>106</v>
+      </c>
+      <c r="I40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E41">
+        <v>230000</v>
+      </c>
+      <c r="F41" t="s">
+        <v>101</v>
+      </c>
+      <c r="G41" t="s">
+        <v>85</v>
+      </c>
+      <c r="H41" t="s">
+        <v>106</v>
+      </c>
+      <c r="I41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1946900</v>
+      </c>
+      <c r="E42">
+        <v>230000</v>
+      </c>
+      <c r="F42" t="s">
+        <v>101</v>
+      </c>
+      <c r="G42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H42" t="s">
+        <v>106</v>
+      </c>
+      <c r="I42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="E43">
+        <v>230000</v>
+      </c>
+      <c r="F43" t="s">
+        <v>101</v>
+      </c>
+      <c r="G43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H43" t="s">
+        <v>106</v>
+      </c>
+      <c r="I43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="E44">
+        <v>230000</v>
+      </c>
+      <c r="F44" t="s">
+        <v>101</v>
+      </c>
+      <c r="G44" t="s">
+        <v>85</v>
+      </c>
+      <c r="H44" t="s">
+        <v>106</v>
+      </c>
+      <c r="I44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" s="4"/>
+      <c r="E45">
+        <v>230000</v>
+      </c>
+      <c r="F45" t="s">
+        <v>101</v>
+      </c>
+      <c r="G45" t="s">
+        <v>85</v>
+      </c>
+      <c r="H45" t="s">
+        <v>106</v>
+      </c>
+      <c r="I45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E46">
+        <v>230000</v>
+      </c>
+      <c r="F46" t="s">
+        <v>101</v>
+      </c>
+      <c r="G46" t="s">
+        <v>85</v>
+      </c>
+      <c r="H46" t="s">
+        <v>106</v>
+      </c>
+      <c r="I46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>107</v>
+      </c>
+      <c r="E47">
+        <v>230000</v>
+      </c>
+      <c r="F47" t="s">
+        <v>101</v>
+      </c>
+      <c r="G47" t="s">
+        <v>85</v>
+      </c>
+      <c r="H47" t="s">
+        <v>106</v>
+      </c>
+      <c r="I47" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B33:B34"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2" display="NNPDF30_nlo_nf_5_pdfas"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F6" r:id="rId4"/>
-    <hyperlink ref="F7" r:id="rId5"/>
-    <hyperlink ref="B8" r:id="rId6"/>
-    <hyperlink ref="B10" r:id="rId7"/>
-    <hyperlink ref="F8" r:id="rId8"/>
-    <hyperlink ref="F9" r:id="rId9"/>
-    <hyperlink ref="F10" r:id="rId10"/>
-    <hyperlink ref="B11" r:id="rId11" display="/TTWJetsToQQ_TuneCUETP8M1_13TeV-amcatnloFXFX-madspin-pythia8/RunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1/MINIAODSIM"/>
-    <hyperlink ref="B12" r:id="rId12"/>
-    <hyperlink ref="B13" r:id="rId13"/>
-    <hyperlink ref="F11" r:id="rId14"/>
-    <hyperlink ref="F12" r:id="rId15"/>
-    <hyperlink ref="F13" r:id="rId16"/>
-    <hyperlink ref="F14" r:id="rId17"/>
-    <hyperlink ref="F15" r:id="rId18"/>
-    <hyperlink ref="F16" r:id="rId19"/>
-    <hyperlink ref="B17" r:id="rId20"/>
-    <hyperlink ref="F17" r:id="rId21"/>
-    <hyperlink ref="F18" r:id="rId22"/>
-    <hyperlink ref="F19" r:id="rId23"/>
-    <hyperlink ref="F20" r:id="rId24"/>
-    <hyperlink ref="F21" r:id="rId25"/>
-    <hyperlink ref="F22" r:id="rId26"/>
-    <hyperlink ref="F23" r:id="rId27"/>
-    <hyperlink ref="F24" r:id="rId28"/>
-    <hyperlink ref="F25" r:id="rId29"/>
-    <hyperlink ref="F26" r:id="rId30"/>
-    <hyperlink ref="F27" r:id="rId31"/>
-    <hyperlink ref="F28" r:id="rId32"/>
-    <hyperlink ref="B30" r:id="rId33"/>
-    <hyperlink ref="B31" r:id="rId34"/>
-    <hyperlink ref="B32" r:id="rId35" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FDYJetsToLL_M-50_TuneCUETP8M1_13TeV-amcatnloFXFX-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_HCALDebug_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
-    <hyperlink ref="B34" r:id="rId36" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FDYJetsToLL_M-50_TuneCUETP8M1_13TeV-amcatnloFXFX-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6_ext2-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
-    <hyperlink ref="B35" r:id="rId37" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FDYJetsToLL_M-10to50_TuneCUETP8M1_13TeV-amcatnloFXFX-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v2%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
-    <hyperlink ref="B36" r:id="rId38" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FDYJetsToLL_M-10to50_TuneCUETP8M1_13TeV-amcatnloFXFX-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6_ext1-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
-    <hyperlink ref="F32" r:id="rId39"/>
-    <hyperlink ref="F33" r:id="rId40"/>
-    <hyperlink ref="F34" r:id="rId41"/>
-    <hyperlink ref="F35" r:id="rId42"/>
+    <hyperlink ref="F6" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2" display="NNPDF30_nlo_nf_5_pdfas"/>
+    <hyperlink ref="F5" r:id="rId3"/>
+    <hyperlink ref="F7" r:id="rId4"/>
+    <hyperlink ref="F8" r:id="rId5"/>
+    <hyperlink ref="B9" r:id="rId6"/>
+    <hyperlink ref="B11" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="F10" r:id="rId9"/>
+    <hyperlink ref="F11" r:id="rId10"/>
+    <hyperlink ref="B12" r:id="rId11" display="/TTWJetsToQQ_TuneCUETP8M1_13TeV-amcatnloFXFX-madspin-pythia8/RunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1/MINIAODSIM"/>
+    <hyperlink ref="B13" r:id="rId12"/>
+    <hyperlink ref="B14" r:id="rId13"/>
+    <hyperlink ref="F12" r:id="rId14"/>
+    <hyperlink ref="F13" r:id="rId15"/>
+    <hyperlink ref="F14" r:id="rId16"/>
+    <hyperlink ref="F15" r:id="rId17"/>
+    <hyperlink ref="F16" r:id="rId18"/>
+    <hyperlink ref="F17" r:id="rId19"/>
+    <hyperlink ref="B18" r:id="rId20"/>
+    <hyperlink ref="F18" r:id="rId21"/>
+    <hyperlink ref="F19" r:id="rId22"/>
+    <hyperlink ref="F20" r:id="rId23"/>
+    <hyperlink ref="F21" r:id="rId24"/>
+    <hyperlink ref="F22" r:id="rId25"/>
+    <hyperlink ref="F23" r:id="rId26"/>
+    <hyperlink ref="F24" r:id="rId27"/>
+    <hyperlink ref="F25" r:id="rId28"/>
+    <hyperlink ref="F26" r:id="rId29"/>
+    <hyperlink ref="F27" r:id="rId30"/>
+    <hyperlink ref="F28" r:id="rId31"/>
+    <hyperlink ref="F29" r:id="rId32"/>
+    <hyperlink ref="B31" r:id="rId33"/>
+    <hyperlink ref="B32" r:id="rId34"/>
+    <hyperlink ref="B33" r:id="rId35" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FDYJetsToLL_M-50_TuneCUETP8M1_13TeV-amcatnloFXFX-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_HCALDebug_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
+    <hyperlink ref="B35" r:id="rId36" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FDYJetsToLL_M-50_TuneCUETP8M1_13TeV-amcatnloFXFX-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6_ext2-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
+    <hyperlink ref="B36" r:id="rId37" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FDYJetsToLL_M-10to50_TuneCUETP8M1_13TeV-amcatnloFXFX-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v2%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
+    <hyperlink ref="B37" r:id="rId38" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FDYJetsToLL_M-10to50_TuneCUETP8M1_13TeV-amcatnloFXFX-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6_ext1-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
+    <hyperlink ref="F33" r:id="rId39"/>
+    <hyperlink ref="F34" r:id="rId40"/>
+    <hyperlink ref="F35" r:id="rId41"/>
+    <hyperlink ref="F36" r:id="rId42"/>
+    <hyperlink ref="F37" r:id="rId43"/>
+    <hyperlink ref="B39" r:id="rId44" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FST_FCNC-TLL_Thadronic_zeta_zct-MadGraph5-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
+    <hyperlink ref="B42" r:id="rId45" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FST_FCNC-TLL_Thadronic_kappa_zut-MadGraph5-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
+    <hyperlink ref="B41" r:id="rId46" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FST_FCNC-TLL_Thadronic_zeta_zut-MadGraph5-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
+    <hyperlink ref="B40" r:id="rId47" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FST_FCNC-TLL_Thadronic_kappa_zct-MadGraph5-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
+    <hyperlink ref="B43" r:id="rId48" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FST_FCNC-TLL_Tleptonic_zeta_zct-MadGraph5-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
+    <hyperlink ref="B44" r:id="rId49" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FST_FCNC-TLL_Tleptonic_kappa_zct-MadGraph5-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
+    <hyperlink ref="B45" r:id="rId50" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FST_FCNC-TLL_Tleptonic_zeta_zut-MadGraph5-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
+    <hyperlink ref="B46" r:id="rId51" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FST_FCNC-TLL_Tleptonic_kappa_zut-MadGraph5-pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
+    <hyperlink ref="B3" r:id="rId52" display="https://cmsweb.cern.ch/das/request?input=dataset%3D%2FtZq_W_lept_Z_hadron_4f_ckm_NLO_13TeV_amcatnlo_pythia8%2FRunIISummer16MiniAODv2-PUMoriond17_80X_mcRun2_asymptotic_2016_TrancheIV_v6-v1%2FMINIAODSIM&amp;instance=prod%2Fglobal"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId43"/>
-  <drawing r:id="rId44"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId53"/>
+  <drawing r:id="rId54"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>